<commit_message>
effect changes on customer and survey template/model
</commit_message>
<xml_diff>
--- a/PMAPortal.Web/wwwroot/templates/MOS Customer Upload Template.xlsx
+++ b/PMAPortal.Web/wwwroot/templates/MOS Customer Upload Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariofrancis\source\repos\PMAPortal\PMAPortal.Web\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73CA51CC-4CE0-492A-950F-C1FCA364C67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBF2F7F-5116-43FA-89C3-62D9F0EBB50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6585" yWindow="1170" windowWidth="16560" windowHeight="13125" xr2:uid="{9E0099B6-6A28-4EAF-8B33-70389F48D491}"/>
+    <workbookView xWindow="12930" yWindow="615" windowWidth="12105" windowHeight="13125" xr2:uid="{9E0099B6-6A28-4EAF-8B33-70389F48D491}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>SN</t>
   </si>
@@ -68,6 +68,24 @@
   </si>
   <si>
     <t>Landmark</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>Feeder</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>Tariff</t>
+  </si>
+  <si>
+    <t>Metered  Status</t>
   </si>
 </sst>
 </file>
@@ -428,11 +446,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05844E02-1A24-423A-89FB-0A317377326A}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -442,9 +458,10 @@
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,6 +497,24 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement admin pages for batch, batch customers and customers
</commit_message>
<xml_diff>
--- a/PMAPortal.Web/wwwroot/templates/MOS Customer Upload Template.xlsx
+++ b/PMAPortal.Web/wwwroot/templates/MOS Customer Upload Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariofrancis\source\repos\PMAPortal\PMAPortal.Web\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBF2F7F-5116-43FA-89C3-62D9F0EBB50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC45C414-5903-407C-A3C4-95A5467D4DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12930" yWindow="615" windowWidth="12105" windowHeight="13125" xr2:uid="{9E0099B6-6A28-4EAF-8B33-70389F48D491}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>Tariff</t>
   </si>
   <si>
-    <t>Metered  Status</t>
+    <t>Metered Status</t>
   </si>
 </sst>
 </file>
@@ -129,9 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,17 +449,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05844E02-1A24-423A-89FB-0A317377326A}">
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="16.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="17.28515625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="15.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="13.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
+    <col min="13" max="17" width="9.140625" style="2"/>
+    <col min="18" max="18" width="19.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>